<commit_message>
Commit Geral dos trabalhos BI-Master
</commit_message>
<xml_diff>
--- a/Desafios-NLP/2021-03-NER/Resultados.xlsx
+++ b/Desafios-NLP/2021-03-NER/Resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bi-master\Desafios-NLP\2021-03-NER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2CE6D1-9D2C-479B-AE2D-FA830263B6A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D58D86-506C-4B4B-9537-9C13DF3CACE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9C2D6089-A465-4ED9-B9D0-35DDAE676677}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>Embedding</t>
   </si>
@@ -88,13 +88,16 @@
   </si>
   <si>
     <t>Lowercase</t>
+  </si>
+  <si>
+    <t>Pubmed PMC Adaptado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +107,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -146,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -157,6 +168,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA99D9F-4D87-4216-BDB1-C58472C1C0C8}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -640,65 +655,65 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3">
+        <v>84.59</v>
+      </c>
+      <c r="D7" s="3">
+        <v>80.180000000000007</v>
+      </c>
+      <c r="E7" s="3">
+        <v>82.33</v>
+      </c>
+      <c r="F7" s="3">
+        <v>75.260000000000005</v>
+      </c>
+      <c r="G7" s="3">
+        <v>72.05</v>
+      </c>
+      <c r="H7" s="3">
+        <v>73.62</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3">
-        <v>75.05</v>
-      </c>
-      <c r="D8" s="3">
-        <v>73.14</v>
-      </c>
-      <c r="E8" s="3">
-        <v>74.08</v>
-      </c>
-      <c r="F8" s="3">
-        <v>70</v>
-      </c>
-      <c r="G8" s="3">
-        <v>70.78</v>
-      </c>
-      <c r="H8" s="3">
-        <v>69.36</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="3">
-        <v>72.150000000000006</v>
+        <v>75.05</v>
       </c>
       <c r="D9" s="3">
-        <v>74.58</v>
+        <v>73.14</v>
       </c>
       <c r="E9" s="3">
-        <v>73.34</v>
+        <v>74.08</v>
       </c>
       <c r="F9" s="3">
-        <v>65.23</v>
+        <v>70</v>
       </c>
       <c r="G9" s="3">
-        <v>72.17</v>
+        <v>70.78</v>
       </c>
       <c r="H9" s="3">
-        <v>68.52</v>
+        <v>69.36</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -706,200 +721,262 @@
         <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="3">
+        <v>72.150000000000006</v>
+      </c>
+      <c r="D10" s="3">
+        <v>74.58</v>
+      </c>
+      <c r="E10" s="3">
+        <v>73.34</v>
+      </c>
+      <c r="F10" s="3">
+        <v>65.23</v>
+      </c>
+      <c r="G10" s="3">
+        <v>72.17</v>
+      </c>
+      <c r="H10" s="3">
+        <v>68.52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C11" s="3">
         <v>75.5</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="3">
         <v>71.97</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E11" s="3">
         <v>73.7</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F11" s="3">
         <v>69.3</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G11" s="3">
         <v>69.91</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H11" s="3">
         <v>69.599999999999994</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3">
+        <v>77.14</v>
+      </c>
+      <c r="D12" s="3">
+        <v>71.010000000000005</v>
+      </c>
+      <c r="E12" s="3">
+        <v>73.95</v>
+      </c>
+      <c r="F12" s="3">
+        <v>69.84</v>
+      </c>
+      <c r="G12" s="3">
+        <v>66.88</v>
+      </c>
+      <c r="H12" s="3">
+        <v>68.33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C15" s="3">
         <v>84.41</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D15" s="3">
         <v>76.28</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E15" s="3">
         <v>80.14</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F15" s="3">
         <v>85.47</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G15" s="3">
         <v>76.12</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H15" s="3">
         <v>80.53</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="3">
-        <v>80.97</v>
-      </c>
-      <c r="D13" s="3">
-        <v>79.16</v>
-      </c>
-      <c r="E13" s="3">
-        <v>80.06</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="3">
-        <v>82.22</v>
-      </c>
-      <c r="D14" s="3">
-        <v>79.319999999999993</v>
-      </c>
-      <c r="E14" s="3">
-        <v>80.739999999999995</v>
-      </c>
-      <c r="F14" s="3">
-        <v>82.8</v>
-      </c>
-      <c r="G14" s="3">
-        <v>79.150000000000006</v>
-      </c>
-      <c r="H14" s="3">
-        <v>80.930000000000007</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" s="3">
-        <v>80.62</v>
+        <v>80.97</v>
       </c>
       <c r="D16" s="3">
-        <v>72.14</v>
+        <v>79.16</v>
       </c>
       <c r="E16" s="3">
-        <v>76.150000000000006</v>
-      </c>
-      <c r="F16" s="3">
-        <v>80.040000000000006</v>
-      </c>
-      <c r="G16" s="3">
-        <v>71.599999999999994</v>
-      </c>
-      <c r="H16" s="3">
-        <v>75.58</v>
+        <v>80.06</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="3">
+        <v>82.22</v>
+      </c>
+      <c r="D17" s="3">
+        <v>79.319999999999993</v>
+      </c>
+      <c r="E17" s="3">
+        <v>80.739999999999995</v>
+      </c>
+      <c r="F17" s="3">
+        <v>82.8</v>
+      </c>
+      <c r="G17" s="3">
+        <v>79.150000000000006</v>
+      </c>
+      <c r="H17" s="3">
+        <v>80.930000000000007</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3">
+        <v>80.62</v>
+      </c>
+      <c r="D19" s="3">
+        <v>72.14</v>
+      </c>
+      <c r="E19" s="3">
+        <v>76.150000000000006</v>
+      </c>
+      <c r="F19" s="3">
+        <v>80.040000000000006</v>
+      </c>
+      <c r="G19" s="3">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="H19" s="3">
+        <v>75.58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C20" s="3">
         <v>77.77</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D20" s="3">
         <v>73.12</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E20" s="3">
         <v>75.37</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F20" s="3">
         <v>76.3</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G20" s="3">
         <v>72.599999999999994</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H20" s="3">
         <v>74.400000000000006</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="21" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C21" s="3">
         <v>76.92</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D21" s="3">
         <v>73.040000000000006</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E21" s="3">
         <v>74.930000000000007</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F21" s="3">
         <v>76.06</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G21" s="3">
         <v>73.290000000000006</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H21" s="3">
         <v>74.650000000000006</v>
       </c>
     </row>

</xml_diff>